<commit_message>
move old data to archive folder
</commit_message>
<xml_diff>
--- a/Team_Bration_Tasks.xlsx
+++ b/Team_Bration_Tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>Task</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>lgoychev: done; nrayanov: done</t>
-  </si>
-  <si>
-    <t>in progress</t>
   </si>
   <si>
     <r>
@@ -558,7 +555,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -599,7 +596,7 @@
         <v>21</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -644,13 +641,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -661,13 +658,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -675,7 +672,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>4</v>
@@ -684,7 +681,7 @@
         <v>21</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -701,7 +698,7 @@
         <v>21</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -718,7 +715,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -735,7 +732,7 @@
         <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -759,8 +756,8 @@
       <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>25</v>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -772,10 +769,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -784,13 +781,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>25</v>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -801,8 +798,12 @@
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -815,8 +816,8 @@
       <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>25</v>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -825,13 +826,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>25</v>
+      <c r="D17" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -840,13 +841,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>25</v>
+      <c r="D18" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -857,9 +858,11 @@
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
-        <v>25</v>
+      <c r="C19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -870,8 +873,12 @@
       <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
+      <c r="C20" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -881,8 +888,12 @@
       <c r="B21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">

</xml_diff>